<commit_message>
fixed bug for age group weights
</commit_message>
<xml_diff>
--- a/excel-files/ASK-2024-Komuna-Gjinia-Mosha.xlsx
+++ b/excel-files/ASK-2024-Komuna-Gjinia-Mosha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Documents\2025\Innovation\sample-automatization\excel-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFA3FC4-AE9A-4D6D-9BA8-556A0E5F35BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69902DE-B5D5-42A5-8E72-F5A35F401AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="census_00" sheetId="2" r:id="rId1"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FT77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BX38" workbookViewId="0">
-      <selection activeCell="CJ50" sqref="CJ50"/>
+    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="CJ1" sqref="CJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>